<commit_message>
Updated doc to section 5.3
</commit_message>
<xml_diff>
--- a/Documentation/Project_Planning/ARPEGOS Costes.xlsx
+++ b/Documentation/Project_Planning/ARPEGOS Costes.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E0D9783-5409-4DD4-887A-60452C95BB71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARPEGOS_Project\Documentation\Project_Planning\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251B7529-9090-4FDE-A058-5CC5B334BE4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Costes Humanos" sheetId="1" r:id="rId1"/>
     <sheet name="Costes Materiales" sheetId="2" r:id="rId2"/>
     <sheet name="Costes Proyecto" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
   <si>
     <t>Actividad</t>
   </si>
@@ -65,9 +70,6 @@
     <t>Tester</t>
   </si>
   <si>
-    <t>Documentador</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -92,9 +94,6 @@
     <t>Ordenador de trabajo</t>
   </si>
   <si>
-    <t>Coste medio luz/día</t>
-  </si>
-  <si>
     <t>Software</t>
   </si>
   <si>
@@ -144,6 +143,12 @@
   </si>
   <si>
     <t>Costes Materiales</t>
+  </si>
+  <si>
+    <t>Documentalist</t>
+  </si>
+  <si>
+    <t>Coste medio luz mensual</t>
   </si>
 </sst>
 </file>
@@ -155,7 +160,7 @@
     <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,7 +329,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -370,11 +375,17 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="9"/>
     <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="8"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="40% - Énfasis1" xfId="5" builtinId="31"/>
@@ -402,7 +413,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -700,11 +711,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
     <col min="2" max="2" width="36.5703125" style="1" customWidth="1"/>
@@ -712,13 +723,13 @@
     <col min="4" max="4" width="27.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" style="12" customWidth="1"/>
     <col min="8" max="8" width="25" style="1" customWidth="1"/>
     <col min="9" max="9" width="18.5703125" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -737,7 +748,7 @@
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -747,7 +758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -757,7 +768,7 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="24" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="1">
@@ -767,7 +778,7 @@
       <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="12">
         <v>32417</v>
       </c>
       <c r="H2" s="10">
@@ -779,7 +790,7 @@
         <v>77.183333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -799,7 +810,7 @@
       <c r="F3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="12">
         <v>31700</v>
       </c>
       <c r="H3" s="10">
@@ -807,11 +818,11 @@
         <v>2264.2857142857142</v>
       </c>
       <c r="I3" s="10">
-        <f t="shared" ref="I3:I6" si="1">H3/30</f>
+        <f t="shared" ref="I3:I7" si="1">H3/30</f>
         <v>75.476190476190467</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -821,7 +832,7 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="25" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="1">
@@ -831,7 +842,7 @@
       <c r="F4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="12">
         <v>26600</v>
       </c>
       <c r="H4" s="10">
@@ -843,7 +854,7 @@
         <v>63.333333333333336</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -863,7 +874,7 @@
       <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="12">
         <v>27138</v>
       </c>
       <c r="H5" s="10">
@@ -875,7 +886,7 @@
         <v>64.614285714285714</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -895,7 +906,7 @@
       <c r="F6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="12">
         <v>26324</v>
       </c>
       <c r="H6" s="10">
@@ -907,7 +918,7 @@
         <v>62.676190476190477</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -918,17 +929,28 @@
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E7" s="1">
         <f>SUM(C27:C29)</f>
         <v>9</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="F7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="12">
+        <v>31165</v>
+      </c>
+      <c r="H7" s="10">
+        <f>G7/14</f>
+        <v>2226.0714285714284</v>
+      </c>
+      <c r="I7" s="10">
+        <f t="shared" si="1"/>
+        <v>74.202380952380949</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -946,7 +968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -957,14 +979,14 @@
         <v>71</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="1">
         <f>SUM(E2:E8)</f>
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -975,7 +997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -989,10 +1011,10 @@
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1002,15 +1024,15 @@
       <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>7</v>
+      <c r="D12" s="24" t="s">
+        <v>6</v>
       </c>
       <c r="E12" s="12">
         <f>PRODUCT(E2,I2)</f>
         <v>231.55</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1028,12 +1050,12 @@
         <v>11925.238095238094</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -1047,12 +1069,12 @@
       </c>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -1065,7 +1087,7 @@
         <v>2196.8857142857141</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1083,7 +1105,7 @@
         <v>250.70476190476191</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1093,15 +1115,15 @@
       <c r="C17" s="3">
         <v>15</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="22">
-        <f>SUM(E12:E16)</f>
-        <v>14921.045238095236</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="D17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="12">
+        <f>PRODUCT(E7,I7)</f>
+        <v>667.82142857142856</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1111,8 +1133,15 @@
       <c r="C18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="D18" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="21">
+        <f>SUM(E12:E17)</f>
+        <v>15588.866666666665</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1123,7 +1152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1134,7 +1163,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1145,7 +1174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1156,7 +1185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1167,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1178,7 +1207,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1189,7 +1218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1200,45 +1229,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C29" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E2:E3 E7:E8" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1246,11 +1279,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528A5538-19CC-40AC-9A9F-54B7C795D150}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" style="15" customWidth="1"/>
@@ -1258,65 +1291,64 @@
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" style="15" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>19</v>
       </c>
       <c r="I1" s="15">
         <v>0.86829999999999996</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="15">
         <f>E3</f>
         <v>345</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="15">
         <v>345</v>
       </c>
       <c r="F2" s="15"/>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="I2">
-        <f>PRODUCT(I1,8)</f>
-        <v>6.9463999999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>56.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="15">
         <f>E12</f>
         <v>0</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E3" s="15">
         <f>SUM(E2)</f>
@@ -1324,148 +1356,149 @@
       </c>
       <c r="F3" s="15"/>
       <c r="H3" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I3" s="15">
-        <f>PRODUCT(I2,215)</f>
-        <v>1493.4759999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <f>PRODUCT(I2/30,215)</f>
+        <v>403.48333333333329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="15">
         <f>E17</f>
-        <v>2013.4759999999999</v>
+        <v>761.81666666666661</v>
       </c>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="20">
         <f>SUM(B2:B4)</f>
-        <v>2358.4759999999997</v>
+        <v>1106.8166666666666</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I5" s="15">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" s="15">
         <v>0</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I6" s="15">
-        <f>PRODUCT(I5,8)</f>
-        <v>520</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <f>PRODUCT(I5/30,215)</f>
+        <v>358.33333333333337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E9" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E10" s="15">
         <v>0</v>
       </c>
       <c r="F10" s="15"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E11" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E12" s="15">
         <f>SUM(E6:E11)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" s="17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E15" s="15">
         <f>I3</f>
-        <v>1493.4759999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>403.48333333333329</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E16" s="15">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
+        <f>I6</f>
+        <v>358.33333333333337</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D17" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="21">
+        <v>21</v>
+      </c>
+      <c r="E17" s="23">
         <f>SUM(E15:E16)</f>
-        <v>2013.4759999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5">
+        <v>761.81666666666661</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="30" spans="2:5">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30"/>
       <c r="C30" s="15"/>
     </row>
@@ -1478,49 +1511,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED177B13-1E62-4D43-947C-C70948885A91}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="15">
+        <f>'Costes Humanos'!E18</f>
+        <v>15588.866666666665</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="15">
-        <f>'Costes Humanos'!E17</f>
-        <v>14921.045238095236</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="19" t="s">
-        <v>38</v>
       </c>
       <c r="B3" s="15">
         <f>'Costes Materiales'!B5</f>
-        <v>2358.4759999999997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>1106.8166666666666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="20">
         <f>SUM(B2:B3)</f>
-        <v>17279.521238095236</v>
+        <v>16695.683333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>